<commit_message>
Minor changes and fixed revive.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/quest-items.xlsx
+++ b/resources/data-imports/Items/quest-items.xlsx
@@ -272,7 +272,7 @@
     <t>Ring Crafter's Book</t>
   </si>
   <si>
-    <t>Makes ring crafting slightly easier. (See Skill Modifiers below)</t>
+    <t>Makes ring crafting slightly easier.</t>
   </si>
   <si>
     <t>Ring Crafting</t>
@@ -2258,19 +2258,7 @@
       <c r="AM6">
         <v>0.25</v>
       </c>
-      <c r="AR6">
-        <v>0</v>
-      </c>
       <c r="AU6">
-        <v>0</v>
-      </c>
-      <c r="AW6">
-        <v>0</v>
-      </c>
-      <c r="AX6">
-        <v>0</v>
-      </c>
-      <c r="AZ6">
         <v>0</v>
       </c>
       <c r="BA6">

</xml_diff>

<commit_message>
Added Cosmetic Text Setting.
- Various Fixes
- Chat Tabs are now drop down for smaller screens.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/quest-items.xlsx
+++ b/resources/data-imports/Items/quest-items.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="397">
   <si>
     <t>id</t>
   </si>
@@ -1188,6 +1188,24 @@
   </si>
   <si>
     <t>The gem on this necklace holds a single memory, once you cannot tap into, but one another might be able to.</t>
+  </si>
+  <si>
+    <t>Lost Tome Of Spells</t>
+  </si>
+  <si>
+    <t>A lost tome The Witch was looking for.</t>
+  </si>
+  <si>
+    <t>Clean White Feather</t>
+  </si>
+  <si>
+    <t>A single clean white feather the Dungeon Master is searching for.</t>
+  </si>
+  <si>
+    <t>Ratty Toy Bear</t>
+  </si>
+  <si>
+    <t>Given to you by the Dungeon Master for the Clean White Feather. A memory of your own past.</t>
   </si>
 </sst>
 </file>
@@ -1527,7 +1545,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BS145"/>
+  <dimension ref="A1:BS148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1976,7 +1994,19 @@
       <c r="AM3">
         <v>0.25</v>
       </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
       <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AZ3">
         <v>0</v>
       </c>
       <c r="BA3">
@@ -2258,7 +2288,19 @@
       <c r="AM6">
         <v>0.25</v>
       </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
       <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>0</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AZ6">
         <v>0</v>
       </c>
       <c r="BA6">
@@ -15395,6 +15437,117 @@
         <v>0</v>
       </c>
       <c r="BP145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:71">
+      <c r="A146">
+        <v>988</v>
+      </c>
+      <c r="C146" t="s">
+        <v>391</v>
+      </c>
+      <c r="D146" t="s">
+        <v>72</v>
+      </c>
+      <c r="F146" t="s">
+        <v>392</v>
+      </c>
+      <c r="AB146">
+        <v>1</v>
+      </c>
+      <c r="AU146">
+        <v>0</v>
+      </c>
+      <c r="BG146">
+        <v>34</v>
+      </c>
+      <c r="BL146">
+        <v>0</v>
+      </c>
+      <c r="BM146">
+        <v>0</v>
+      </c>
+      <c r="BN146">
+        <v>0</v>
+      </c>
+      <c r="BO146">
+        <v>0</v>
+      </c>
+      <c r="BP146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:71">
+      <c r="A147">
+        <v>989</v>
+      </c>
+      <c r="C147" t="s">
+        <v>393</v>
+      </c>
+      <c r="D147" t="s">
+        <v>72</v>
+      </c>
+      <c r="F147" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB147">
+        <v>1</v>
+      </c>
+      <c r="AU147">
+        <v>0</v>
+      </c>
+      <c r="BG147">
+        <v>34</v>
+      </c>
+      <c r="BL147">
+        <v>0</v>
+      </c>
+      <c r="BM147">
+        <v>0</v>
+      </c>
+      <c r="BN147">
+        <v>0</v>
+      </c>
+      <c r="BO147">
+        <v>0</v>
+      </c>
+      <c r="BP147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:71">
+      <c r="A148">
+        <v>990</v>
+      </c>
+      <c r="C148" t="s">
+        <v>395</v>
+      </c>
+      <c r="D148" t="s">
+        <v>72</v>
+      </c>
+      <c r="F148" t="s">
+        <v>396</v>
+      </c>
+      <c r="AB148">
+        <v>1</v>
+      </c>
+      <c r="AU148">
+        <v>0</v>
+      </c>
+      <c r="BL148">
+        <v>0</v>
+      </c>
+      <c r="BM148">
+        <v>0</v>
+      </c>
+      <c r="BN148">
+        <v>0</v>
+      </c>
+      <c r="BO148">
+        <v>0</v>
+      </c>
+      <c r="BP148">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lots of changes - tests are failing out and I am not sure why
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/quest-items.xlsx
+++ b/resources/data-imports/Items/quest-items.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="484">
   <si>
     <t>id</t>
   </si>
@@ -1455,6 +1455,18 @@
   </si>
   <si>
     <t>A simple walking stick used by The Poet</t>
+  </si>
+  <si>
+    <t>Rusted Keys</t>
+  </si>
+  <si>
+    <t>A set of keys that once made the frozen wreck move.</t>
+  </si>
+  <si>
+    <t>Husbands Wallet</t>
+  </si>
+  <si>
+    <t>A wallet covered in blood with a single picture of The Creators father</t>
   </si>
 </sst>
 </file>
@@ -1794,7 +1806,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BT181"/>
+  <dimension ref="A1:BT183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -18270,6 +18282,79 @@
         <v>0</v>
       </c>
     </row>
+    <row r="182" spans="1:72">
+      <c r="A182">
+        <v>126997</v>
+      </c>
+      <c r="C182" t="s">
+        <v>480</v>
+      </c>
+      <c r="D182" t="s">
+        <v>73</v>
+      </c>
+      <c r="G182" t="s">
+        <v>481</v>
+      </c>
+      <c r="AC182">
+        <v>1</v>
+      </c>
+      <c r="AV182">
+        <v>0</v>
+      </c>
+      <c r="BH182" t="s">
+        <v>407</v>
+      </c>
+      <c r="BM182">
+        <v>0</v>
+      </c>
+      <c r="BN182">
+        <v>0</v>
+      </c>
+      <c r="BO182">
+        <v>0</v>
+      </c>
+      <c r="BP182">
+        <v>0</v>
+      </c>
+      <c r="BQ182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:72">
+      <c r="A183">
+        <v>126998</v>
+      </c>
+      <c r="C183" t="s">
+        <v>482</v>
+      </c>
+      <c r="D183" t="s">
+        <v>73</v>
+      </c>
+      <c r="G183" t="s">
+        <v>483</v>
+      </c>
+      <c r="AC183">
+        <v>1</v>
+      </c>
+      <c r="AV183">
+        <v>0</v>
+      </c>
+      <c r="BM183">
+        <v>0</v>
+      </c>
+      <c r="BN183">
+        <v>0</v>
+      </c>
+      <c r="BO183">
+        <v>0</v>
+      </c>
+      <c r="BP183">
+        <v>0</v>
+      </c>
+      <c r="BQ183">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removed the mercenaries and tests.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/quest-items.xlsx
+++ b/resources/data-imports/Items/quest-items.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="489">
   <si>
     <t>id</t>
   </si>
@@ -1473,6 +1473,15 @@
   </si>
   <si>
     <t>Allows you to enter: The Old Church (X/Y): 80/256 while on The Ice Plane during The Winter Event.</t>
+  </si>
+  <si>
+    <t>Childs Faceless Idol</t>
+  </si>
+  <si>
+    <t>Given to the children by the church. Toys they were called. Mercenaries they became in the fight against the darkness that crept into a childs dreams. [This item will allow you to gain +50% on currency rewards from slots and additional 5% of copper coins when you are fighting at Purgatory Dungeons]</t>
+  </si>
+  <si>
+    <t>mercenary-slot-bonus</t>
   </si>
 </sst>
 </file>
@@ -1812,7 +1821,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BT184"/>
+  <dimension ref="A1:BT185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -19335,7 +19344,7 @@
     </row>
     <row r="184" spans="1:72">
       <c r="A184">
-        <v>376323</v>
+        <v>410519</v>
       </c>
       <c r="C184" t="s">
         <v>484</v>
@@ -19419,6 +19428,44 @@
         <v>0</v>
       </c>
       <c r="BQ184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:72">
+      <c r="A185">
+        <v>938325</v>
+      </c>
+      <c r="C185" t="s">
+        <v>486</v>
+      </c>
+      <c r="D185" t="s">
+        <v>73</v>
+      </c>
+      <c r="G185" t="s">
+        <v>487</v>
+      </c>
+      <c r="AA185" t="s">
+        <v>488</v>
+      </c>
+      <c r="AC185">
+        <v>1</v>
+      </c>
+      <c r="AV185">
+        <v>0</v>
+      </c>
+      <c r="BM185">
+        <v>0</v>
+      </c>
+      <c r="BN185">
+        <v>0</v>
+      </c>
+      <c r="BO185">
+        <v>0</v>
+      </c>
+      <c r="BP185">
+        <v>0</v>
+      </c>
+      <c r="BQ185">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More changes - new quests for the new plane.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/quest-items.xlsx
+++ b/resources/data-imports/Items/quest-items.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="491">
   <si>
     <t>id</t>
   </si>
@@ -1482,6 +1482,12 @@
   </si>
   <si>
     <t>mercenary-slot-bonus</t>
+  </si>
+  <si>
+    <t>Twisted Tree Branch</t>
+  </si>
+  <si>
+    <t>With this item players can enter the Twisted Diemsional Gate in Hell to be automatically taken to the Twisted Memories plane. No traversing required.</t>
   </si>
 </sst>
 </file>
@@ -1821,7 +1827,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BT185"/>
+  <dimension ref="A1:BT186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -19433,7 +19439,7 @@
     </row>
     <row r="185" spans="1:72">
       <c r="A185">
-        <v>938325</v>
+        <v>938213</v>
       </c>
       <c r="C185" t="s">
         <v>486</v>
@@ -19444,15 +19450,69 @@
       <c r="G185" t="s">
         <v>487</v>
       </c>
+      <c r="O185">
+        <v>0</v>
+      </c>
+      <c r="Y185">
+        <v>0</v>
+      </c>
+      <c r="Z185">
+        <v>0</v>
+      </c>
       <c r="AA185" t="s">
         <v>488</v>
       </c>
       <c r="AC185">
         <v>1</v>
       </c>
+      <c r="AI185">
+        <v>0</v>
+      </c>
+      <c r="AJ185">
+        <v>0</v>
+      </c>
+      <c r="AK185">
+        <v>0</v>
+      </c>
+      <c r="AL185">
+        <v>0</v>
+      </c>
+      <c r="AM185">
+        <v>0</v>
+      </c>
+      <c r="AS185">
+        <v>0</v>
+      </c>
       <c r="AV185">
         <v>0</v>
       </c>
+      <c r="AX185">
+        <v>0</v>
+      </c>
+      <c r="AY185">
+        <v>0</v>
+      </c>
+      <c r="BA185">
+        <v>0</v>
+      </c>
+      <c r="BB185">
+        <v>0</v>
+      </c>
+      <c r="BC185">
+        <v>0</v>
+      </c>
+      <c r="BD185">
+        <v>0</v>
+      </c>
+      <c r="BE185">
+        <v>0</v>
+      </c>
+      <c r="BF185">
+        <v>0</v>
+      </c>
+      <c r="BG185">
+        <v>0</v>
+      </c>
       <c r="BM185">
         <v>0</v>
       </c>
@@ -19466,6 +19526,41 @@
         <v>0</v>
       </c>
       <c r="BQ185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:72">
+      <c r="A186">
+        <v>938214</v>
+      </c>
+      <c r="C186" t="s">
+        <v>489</v>
+      </c>
+      <c r="D186" t="s">
+        <v>73</v>
+      </c>
+      <c r="G186" t="s">
+        <v>490</v>
+      </c>
+      <c r="AC186">
+        <v>1</v>
+      </c>
+      <c r="AV186">
+        <v>0</v>
+      </c>
+      <c r="BM186">
+        <v>0</v>
+      </c>
+      <c r="BN186">
+        <v>0</v>
+      </c>
+      <c r="BO186">
+        <v>0</v>
+      </c>
+      <c r="BP186">
+        <v>0</v>
+      </c>
+      <c r="BQ186">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a new way for mobile players to see their active boons.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/quest-items.xlsx
+++ b/resources/data-imports/Items/quest-items.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="507">
   <si>
     <t>id</t>
   </si>
@@ -1488,6 +1488,54 @@
   </si>
   <si>
     <t>With this item players can enter the Twisted Diemsional Gate in Hell to be automatically taken to the Twisted Memories plane. No traversing required.</t>
+  </si>
+  <si>
+    <t>Twisted Dice</t>
+  </si>
+  <si>
+    <t>Dice that you find in the depths of the dungeons. Their rolls and outcome are always twisted to your own delusional desire.</t>
+  </si>
+  <si>
+    <t>Shattered Emerald</t>
+  </si>
+  <si>
+    <t>A single broken emerald. It is carved in such a way that it was decorative, but also had meaning.</t>
+  </si>
+  <si>
+    <t>Torn map of another land</t>
+  </si>
+  <si>
+    <t>The land upon the map does not look famillar to you, It does not seem to be that of the famed land The Wondering Prince comes from, the one you seek. It seems to be of another more distant land.</t>
+  </si>
+  <si>
+    <t>Tear of the shade</t>
+  </si>
+  <si>
+    <t>A single tear from The Shadoe Lord.</t>
+  </si>
+  <si>
+    <t>Faceless Robe</t>
+  </si>
+  <si>
+    <t>A faceless robe worn by a faceless man who people say is The Wondering Prince.</t>
+  </si>
+  <si>
+    <t>Bottle of missery</t>
+  </si>
+  <si>
+    <t>Drink away the sorrows of the past and refuse to accept the fate that is before you.</t>
+  </si>
+  <si>
+    <t>The princes ring</t>
+  </si>
+  <si>
+    <t>A ring given to The Soldier who lost it sometime ago. A ring given to him by The Wondering Prince.</t>
+  </si>
+  <si>
+    <t>Ashes of the shade</t>
+  </si>
+  <si>
+    <t>Ashes that the Child of Shade holds on to. Why?</t>
   </si>
 </sst>
 </file>
@@ -1827,7 +1875,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BT186"/>
+  <dimension ref="A1:BT194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -19564,6 +19612,310 @@
         <v>0</v>
       </c>
     </row>
+    <row r="187" spans="1:72">
+      <c r="A187">
+        <v>938215</v>
+      </c>
+      <c r="C187" t="s">
+        <v>491</v>
+      </c>
+      <c r="D187" t="s">
+        <v>73</v>
+      </c>
+      <c r="G187" t="s">
+        <v>492</v>
+      </c>
+      <c r="AC187">
+        <v>1</v>
+      </c>
+      <c r="AV187">
+        <v>0</v>
+      </c>
+      <c r="BH187" t="s">
+        <v>166</v>
+      </c>
+      <c r="BM187">
+        <v>0</v>
+      </c>
+      <c r="BN187">
+        <v>0</v>
+      </c>
+      <c r="BO187">
+        <v>0</v>
+      </c>
+      <c r="BP187">
+        <v>0</v>
+      </c>
+      <c r="BQ187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:72">
+      <c r="A188">
+        <v>938216</v>
+      </c>
+      <c r="C188" t="s">
+        <v>493</v>
+      </c>
+      <c r="D188" t="s">
+        <v>73</v>
+      </c>
+      <c r="G188" t="s">
+        <v>494</v>
+      </c>
+      <c r="AC188">
+        <v>1</v>
+      </c>
+      <c r="AV188">
+        <v>0</v>
+      </c>
+      <c r="BH188" t="s">
+        <v>166</v>
+      </c>
+      <c r="BM188">
+        <v>0</v>
+      </c>
+      <c r="BN188">
+        <v>0</v>
+      </c>
+      <c r="BO188">
+        <v>0</v>
+      </c>
+      <c r="BP188">
+        <v>0</v>
+      </c>
+      <c r="BQ188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:72">
+      <c r="A189">
+        <v>938217</v>
+      </c>
+      <c r="C189" t="s">
+        <v>495</v>
+      </c>
+      <c r="D189" t="s">
+        <v>73</v>
+      </c>
+      <c r="G189" t="s">
+        <v>496</v>
+      </c>
+      <c r="AC189">
+        <v>1</v>
+      </c>
+      <c r="AV189">
+        <v>0</v>
+      </c>
+      <c r="BH189" t="s">
+        <v>166</v>
+      </c>
+      <c r="BM189">
+        <v>0</v>
+      </c>
+      <c r="BN189">
+        <v>0</v>
+      </c>
+      <c r="BO189">
+        <v>0</v>
+      </c>
+      <c r="BP189">
+        <v>0</v>
+      </c>
+      <c r="BQ189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:72">
+      <c r="A190">
+        <v>938218</v>
+      </c>
+      <c r="C190" t="s">
+        <v>497</v>
+      </c>
+      <c r="D190" t="s">
+        <v>73</v>
+      </c>
+      <c r="G190" t="s">
+        <v>498</v>
+      </c>
+      <c r="AC190">
+        <v>1</v>
+      </c>
+      <c r="AV190">
+        <v>0</v>
+      </c>
+      <c r="BH190" t="s">
+        <v>172</v>
+      </c>
+      <c r="BM190">
+        <v>0</v>
+      </c>
+      <c r="BN190">
+        <v>0</v>
+      </c>
+      <c r="BO190">
+        <v>0</v>
+      </c>
+      <c r="BP190">
+        <v>0</v>
+      </c>
+      <c r="BQ190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:72">
+      <c r="A191">
+        <v>938219</v>
+      </c>
+      <c r="C191" t="s">
+        <v>499</v>
+      </c>
+      <c r="D191" t="s">
+        <v>73</v>
+      </c>
+      <c r="G191" t="s">
+        <v>500</v>
+      </c>
+      <c r="AC191">
+        <v>1</v>
+      </c>
+      <c r="AV191">
+        <v>0</v>
+      </c>
+      <c r="BH191" t="s">
+        <v>176</v>
+      </c>
+      <c r="BM191">
+        <v>0</v>
+      </c>
+      <c r="BN191">
+        <v>0</v>
+      </c>
+      <c r="BO191">
+        <v>0</v>
+      </c>
+      <c r="BP191">
+        <v>0</v>
+      </c>
+      <c r="BQ191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:72">
+      <c r="A192">
+        <v>938220</v>
+      </c>
+      <c r="C192" t="s">
+        <v>501</v>
+      </c>
+      <c r="D192" t="s">
+        <v>73</v>
+      </c>
+      <c r="G192" t="s">
+        <v>502</v>
+      </c>
+      <c r="AC192">
+        <v>1</v>
+      </c>
+      <c r="AV192">
+        <v>0</v>
+      </c>
+      <c r="BH192" t="s">
+        <v>172</v>
+      </c>
+      <c r="BM192">
+        <v>0</v>
+      </c>
+      <c r="BN192">
+        <v>0</v>
+      </c>
+      <c r="BO192">
+        <v>0</v>
+      </c>
+      <c r="BP192">
+        <v>0</v>
+      </c>
+      <c r="BQ192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:72">
+      <c r="A193">
+        <v>938221</v>
+      </c>
+      <c r="C193" t="s">
+        <v>503</v>
+      </c>
+      <c r="D193" t="s">
+        <v>73</v>
+      </c>
+      <c r="G193" t="s">
+        <v>504</v>
+      </c>
+      <c r="AC193">
+        <v>1</v>
+      </c>
+      <c r="AV193">
+        <v>0</v>
+      </c>
+      <c r="BH193" t="s">
+        <v>176</v>
+      </c>
+      <c r="BM193">
+        <v>0</v>
+      </c>
+      <c r="BN193">
+        <v>0</v>
+      </c>
+      <c r="BO193">
+        <v>0</v>
+      </c>
+      <c r="BP193">
+        <v>0</v>
+      </c>
+      <c r="BQ193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:72">
+      <c r="A194">
+        <v>938222</v>
+      </c>
+      <c r="C194" t="s">
+        <v>505</v>
+      </c>
+      <c r="D194" t="s">
+        <v>73</v>
+      </c>
+      <c r="G194" t="s">
+        <v>506</v>
+      </c>
+      <c r="AC194">
+        <v>1</v>
+      </c>
+      <c r="AV194">
+        <v>0</v>
+      </c>
+      <c r="BH194" t="s">
+        <v>176</v>
+      </c>
+      <c r="BM194">
+        <v>0</v>
+      </c>
+      <c r="BN194">
+        <v>0</v>
+      </c>
+      <c r="BO194">
+        <v>0</v>
+      </c>
+      <c r="BP194">
+        <v>0</v>
+      </c>
+      <c r="BQ194">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated to quest items, locations and quests, location detail changes as well
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/quest-items.xlsx
+++ b/resources/data-imports/Items/quest-items.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="708">
   <si>
     <t>id</t>
   </si>
@@ -242,6 +242,66 @@
     <t>There is a ship, high in the sky, driven by a man who wore a ring carved of emeralds from another plane. Another time.</t>
   </si>
   <si>
+    <t>Musty Childs Teddy bare</t>
+  </si>
+  <si>
+    <t>A musty old child's teddy bare that Trix once carried when he watched the Ascension.</t>
+  </si>
+  <si>
+    <t>Church of God</t>
+  </si>
+  <si>
+    <t>Wet Cat Food</t>
+  </si>
+  <si>
+    <t>Wet cat food that Mrs. Piper is obssessed with.</t>
+  </si>
+  <si>
+    <t>Frozen Pet Cemetary</t>
+  </si>
+  <si>
+    <t>Tree Skirt</t>
+  </si>
+  <si>
+    <t>An old ratted christmas tree skirt that is ratted and torn. Cat's generally like to sleep on these things unless of course they are busy tearing the tree down.</t>
+  </si>
+  <si>
+    <t>Gingerbread Cookies</t>
+  </si>
+  <si>
+    <t>These cookies, while old and stale do not taste as such. They taste as if they have come fresh out the oven. warm and soft. They invoke memories of a better time, almost in a magical way.</t>
+  </si>
+  <si>
+    <t>Frozen Queens Bank</t>
+  </si>
+  <si>
+    <t>Isabella’s earrings</t>
+  </si>
+  <si>
+    <t>These earrings were worn by Isabella on the night of the crash. it is said they can show a time when there was closeness between two people. Alas you wonder if the magic has gone out in them.</t>
+  </si>
+  <si>
+    <t>The Frozen Wreck</t>
+  </si>
+  <si>
+    <t>Leather watch</t>
+  </si>
+  <si>
+    <t>An old leather watch that has some significance to an enchanted snowman.</t>
+  </si>
+  <si>
+    <t>Dusty old presents</t>
+  </si>
+  <si>
+    <t>Old presents that were for The Child, gifted by his parents. Gadgets and gizmos. Alas he never saw that christmas and now The Poet, old and haggard searches for them. Why?</t>
+  </si>
+  <si>
+    <t>Bloody Journal</t>
+  </si>
+  <si>
+    <t>A journal that talks of a failed ascension, the jouney to such an ascension and the way The Poet guided The Child, or at least attempted to.</t>
+  </si>
+  <si>
     <t>Christmas Tree Ordainment</t>
   </si>
   <si>
@@ -251,66 +311,6 @@
     <t>Banshee Fields of Tomorrow</t>
   </si>
   <si>
-    <t>Bloody Journal</t>
-  </si>
-  <si>
-    <t>A journal that talks of a failed ascension, the jouney to such an ascension and the way The Poet guided The Child, or at least attempted to.</t>
-  </si>
-  <si>
-    <t>Dusty old presents</t>
-  </si>
-  <si>
-    <t>Old presents that were for The Child, gifted by his parents. Gadgets and gizmos. Alas he never saw that christmas and now The Poet, old and haggard searches for them. Why?</t>
-  </si>
-  <si>
-    <t>The Frozen Wreck</t>
-  </si>
-  <si>
-    <t>Leather watch</t>
-  </si>
-  <si>
-    <t>An old leather watch that has some significance to an enchanted snowman.</t>
-  </si>
-  <si>
-    <t>Isabella’s earrings</t>
-  </si>
-  <si>
-    <t>These earrings were worn by Isabella on the night of the crash. it is said they can show a time when there was closeness between two people. Alas you wonder if the magic has gone out in them.</t>
-  </si>
-  <si>
-    <t>Gingerbread Cookies</t>
-  </si>
-  <si>
-    <t>These cookies, while old and stale do not taste as such. They taste as if they have come fresh out the oven. warm and soft. They invoke memories of a better time, almost in a magical way.</t>
-  </si>
-  <si>
-    <t>Frozen Queens Bank</t>
-  </si>
-  <si>
-    <t>Tree Skirt</t>
-  </si>
-  <si>
-    <t>An old ratted christmas tree skirt that is ratted and torn. Cat's generally like to sleep on these things unless of course they are busy tearing the tree down.</t>
-  </si>
-  <si>
-    <t>Wet Cat Food</t>
-  </si>
-  <si>
-    <t>Wet cat food that Mrs. Piper is obssessed with.</t>
-  </si>
-  <si>
-    <t>Frozen Pet Cemetary</t>
-  </si>
-  <si>
-    <t>Musty Childs Teddy bare</t>
-  </si>
-  <si>
-    <t>A musty old child's teddy bare that Trix once carried when he watched the Ascension.</t>
-  </si>
-  <si>
-    <t>Church of God</t>
-  </si>
-  <si>
     <t>Maidens Twisted Heart</t>
   </si>
   <si>
@@ -407,156 +407,156 @@
     <t>A mysterious journal written by an old man simply known as The River Man</t>
   </si>
   <si>
+    <t>Teddy Bear</t>
+  </si>
+  <si>
+    <t>A childs toy, soft, warm and still somewhat clean.</t>
+  </si>
+  <si>
+    <t>Abandoned Village</t>
+  </si>
+  <si>
+    <t>Bronze Armour</t>
+  </si>
+  <si>
+    <t>Bronze Armour that was worn by The Soldiers father. The Soldier searches for it, probably for sentimental reasons.</t>
+  </si>
+  <si>
+    <t>The Poets Key</t>
+  </si>
+  <si>
+    <t>A key that opens the door to The Poet Frozen House in The Ice Plane. Alas there seems to be more to opening that door then you can imagine. Maybe some dust will happen as well, but not Gold Dust.</t>
+  </si>
+  <si>
+    <t>Two Lumps of Coal</t>
+  </si>
+  <si>
+    <t>Two lumps of coal that are used as eyes by the father of The Soldier and his brother. Eyes made of coal, sounds pretty gruesome. Here you thought lumps of coal were given to naughty children. Least that's what Trix once told you.</t>
+  </si>
+  <si>
+    <t>Cat Bones</t>
+  </si>
+  <si>
+    <t>These bones are all the bones that make up a dead cat. A cat that wwas burried a long time ago in a pet cemetary. Something dug them up and kept them as a treasure.</t>
+  </si>
+  <si>
+    <t>Everlasting Candle</t>
+  </si>
+  <si>
+    <t>This candle never melts the wax, gives off a ton of heat and nothing but you putting it out seems to blow out the flame. You cannot figure out what the magic is that keeps it so "ever lasting" but you realize that someone might need it to see better in the dark.</t>
+  </si>
+  <si>
+    <t>Rusty Laser Pointer</t>
+  </si>
+  <si>
+    <t>an old rusty contraption that shoots a beam of red light at the ground. There is a small red dot that appears on the ground. What could this be used for?</t>
+  </si>
+  <si>
+    <t>Spinner Ball Toy</t>
+  </si>
+  <si>
+    <t>This small ball has a bell in the middle that gently rings as it rolls. You wonder if a cat might like this, or a child?</t>
+  </si>
+  <si>
+    <t>Red and Green Ribbon</t>
+  </si>
+  <si>
+    <t>Looks like something used to decoratively tie up christmas gifts. Its just a small length of red and green ribbon alternating i color.</t>
+  </si>
+  <si>
+    <t>Leather Wallet</t>
+  </si>
+  <si>
+    <t>An old leather wallet that has nothing in it. Who did it belong to?</t>
+  </si>
+  <si>
+    <t>Wool Scarf</t>
+  </si>
+  <si>
+    <t>An warm looking scarf made of grey wool. It could be used to keep warm, but someone else might looking to get warm.</t>
+  </si>
+  <si>
+    <t>Warm Winter Boots</t>
+  </si>
+  <si>
+    <t>These boots are made of leather and fur, they are slightly too big for a child, but far too small for an adult.</t>
+  </si>
+  <si>
+    <t>Hand mirror into the past</t>
+  </si>
+  <si>
+    <t>A single hand mirror that shows you the past, the past of what was and what never was at the same time.</t>
+  </si>
+  <si>
+    <t>Satans Cage</t>
+  </si>
+  <si>
+    <t>Wooden Toy Train</t>
+  </si>
+  <si>
+    <t>Given to children during the cold winter months fro parents who wanted to keep their children inside and warm and busy instead of pestering them. Who could want this?</t>
+  </si>
+  <si>
+    <t>Tuna Fish Wet Food</t>
+  </si>
+  <si>
+    <t>A can of wet food made of tuna. Cat's love fish right?</t>
+  </si>
+  <si>
+    <t>Feathered Wand</t>
+  </si>
+  <si>
+    <t>A simple feathered wand that you know Mr. Whiskers would love to play with! Maybe you should bring it to him and see what joy he gets it from.</t>
+  </si>
+  <si>
+    <t>Locket of her hair</t>
+  </si>
+  <si>
+    <t>A simple locket of a mothers hair, a wifes hair, a hair that belonged to a time of love and hope.</t>
+  </si>
+  <si>
+    <t>Necklace of silver</t>
+  </si>
+  <si>
+    <t>A simple necklace made of silver, a young man once wore this.</t>
+  </si>
+  <si>
+    <t>Golden Pocket Watch</t>
+  </si>
+  <si>
+    <t>A watch that still tells time. A cat wants this so he can look backwards and forwards at what was and what will be. But can cats tell time?</t>
+  </si>
+  <si>
+    <t>Black Fur Coat</t>
+  </si>
+  <si>
+    <t>A simple black fur coat worn when the weather turns bitter and cold.</t>
+  </si>
+  <si>
+    <t>Family Photo</t>
+  </si>
+  <si>
+    <t>A photo of a smiling and loving family. its frame is dirty and busted and glass is chipped and cracked. But you can still make out the imae beneath it all.</t>
+  </si>
+  <si>
+    <t>Dust of broken memories</t>
+  </si>
+  <si>
+    <t>This dust contains the memories of items collected. Memories that can be used against The Frozen King, but how?</t>
+  </si>
+  <si>
+    <t>Shield of Hope</t>
+  </si>
+  <si>
+    <t>A wooden shield imbued with hope. Let it stand against the icy wind of pain and torment that haunts those who you must eventually face.</t>
+  </si>
+  <si>
     <t>Bloody Tunic</t>
   </si>
   <si>
     <t>This tunic, covered in blood shows that someone was stabbed through the stomach, with what loks like a blade of somekind. Could this item bring back the truth of a situation that they are hiding from?</t>
   </si>
   <si>
-    <t>Shield of Hope</t>
-  </si>
-  <si>
-    <t>A wooden shield imbued with hope. Let it stand against the icy wind of pain and torment that haunts those who you must eventually face.</t>
-  </si>
-  <si>
-    <t>Dust of broken memories</t>
-  </si>
-  <si>
-    <t>This dust contains the memories of items collected. Memories that can be used against The Frozen King, but how?</t>
-  </si>
-  <si>
-    <t>Family Photo</t>
-  </si>
-  <si>
-    <t>A photo of a smiling and loving family. its frame is dirty and busted and glass is chipped and cracked. But you can still make out the imae beneath it all.</t>
-  </si>
-  <si>
-    <t>Black Fur Coat</t>
-  </si>
-  <si>
-    <t>A simple black fur coat worn when the weather turns bitter and cold.</t>
-  </si>
-  <si>
-    <t>Golden Pocket Watch</t>
-  </si>
-  <si>
-    <t>A watch that still tells time. A cat wants this so he can look backwards and forwards at what was and what will be. But can cats tell time?</t>
-  </si>
-  <si>
-    <t>Necklace of silver</t>
-  </si>
-  <si>
-    <t>A simple necklace made of silver, a young man once wore this.</t>
-  </si>
-  <si>
-    <t>Locket of her hair</t>
-  </si>
-  <si>
-    <t>A simple locket of a mothers hair, a wifes hair, a hair that belonged to a time of love and hope.</t>
-  </si>
-  <si>
-    <t>Feathered Wand</t>
-  </si>
-  <si>
-    <t>A simple feathered wand that you know Mr. Whiskers would love to play with! Maybe you should bring it to him and see what joy he gets it from.</t>
-  </si>
-  <si>
-    <t>Abandoned Village</t>
-  </si>
-  <si>
-    <t>Tuna Fish Wet Food</t>
-  </si>
-  <si>
-    <t>A can of wet food made of tuna. Cat's love fish right?</t>
-  </si>
-  <si>
-    <t>Wooden Toy Train</t>
-  </si>
-  <si>
-    <t>Given to children during the cold winter months fro parents who wanted to keep their children inside and warm and busy instead of pestering them. Who could want this?</t>
-  </si>
-  <si>
-    <t>Teddy Bear</t>
-  </si>
-  <si>
-    <t>A childs toy, soft, warm and still somewhat clean.</t>
-  </si>
-  <si>
-    <t>Hand mirror into the past</t>
-  </si>
-  <si>
-    <t>A single hand mirror that shows you the past, the past of what was and what never was at the same time.</t>
-  </si>
-  <si>
-    <t>Satans Cage</t>
-  </si>
-  <si>
-    <t>Warm Winter Boots</t>
-  </si>
-  <si>
-    <t>These boots are made of leather and fur, they are slightly too big for a child, but far too small for an adult.</t>
-  </si>
-  <si>
-    <t>Wool Scarf</t>
-  </si>
-  <si>
-    <t>An warm looking scarf made of grey wool. It could be used to keep warm, but someone else might looking to get warm.</t>
-  </si>
-  <si>
-    <t>Leather Wallet</t>
-  </si>
-  <si>
-    <t>An old leather wallet that has nothing in it. Who did it belong to?</t>
-  </si>
-  <si>
-    <t>Red and Green Ribbon</t>
-  </si>
-  <si>
-    <t>Looks like something used to decoratively tie up christmas gifts. Its just a small length of red and green ribbon alternating i color.</t>
-  </si>
-  <si>
-    <t>Spinner Ball Toy</t>
-  </si>
-  <si>
-    <t>This small ball has a bell in the middle that gently rings as it rolls. You wonder if a cat might like this, or a child?</t>
-  </si>
-  <si>
-    <t>Rusty Laser Pointer</t>
-  </si>
-  <si>
-    <t>an old rusty contraption that shoots a beam of red light at the ground. There is a small red dot that appears on the ground. What could this be used for?</t>
-  </si>
-  <si>
-    <t>Everlasting Candle</t>
-  </si>
-  <si>
-    <t>This candle never melts the wax, gives off a ton of heat and nothing but you putting it out seems to blow out the flame. You cannot figure out what the magic is that keeps it so "ever lasting" but you realize that someone might need it to see better in the dark.</t>
-  </si>
-  <si>
-    <t>Cat Bones</t>
-  </si>
-  <si>
-    <t>These bones are all the bones that make up a dead cat. A cat that wwas burried a long time ago in a pet cemetary. Something dug them up and kept them as a treasure.</t>
-  </si>
-  <si>
-    <t>Two Lumps of Coal</t>
-  </si>
-  <si>
-    <t>Two lumps of coal that are used as eyes by the father of The Soldier and his brother. Eyes made of coal, sounds pretty gruesome. Here you thought lumps of coal were given to naughty children. Least that's what Trix once told you.</t>
-  </si>
-  <si>
-    <t>The Poets Key</t>
-  </si>
-  <si>
-    <t>A key that opens the door to The Poet Frozen House in The Ice Plane. Alas there seems to be more to opening that door then you can imagine. Maybe some dust will happen as well, but not Gold Dust.</t>
-  </si>
-  <si>
-    <t>Bronze Armour</t>
-  </si>
-  <si>
-    <t>Bronze Armour that was worn by The Soldiers father. The Soldier searches for it, probably for sentimental reasons.</t>
-  </si>
-  <si>
     <t>Strand of golden hair</t>
   </si>
   <si>
@@ -2070,6 +2070,9 @@
   </si>
   <si>
     <t>Allows you to enter: The Old Church (X/Y): 80/256 while on The Ice Plane during The Winter Event.</t>
+  </si>
+  <si>
+    <t>the-old-church</t>
   </si>
   <si>
     <t>Black and Silver Ever Living Rose</t>
@@ -2866,7 +2869,7 @@
     </row>
     <row r="3" spans="1:72">
       <c r="A3">
-        <v>2394589</v>
+        <v>2406751</v>
       </c>
       <c r="C3" t="s">
         <v>75</v>
@@ -2877,10 +2880,64 @@
       <c r="G3" t="s">
         <v>76</v>
       </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
       <c r="AC3">
         <v>1</v>
       </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
       <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="BA3">
+        <v>0</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3">
+        <v>0</v>
+      </c>
+      <c r="BD3">
+        <v>0</v>
+      </c>
+      <c r="BE3">
+        <v>0</v>
+      </c>
+      <c r="BF3">
+        <v>0</v>
+      </c>
+      <c r="BG3">
         <v>0</v>
       </c>
       <c r="BH3" t="s">
@@ -2904,7 +2961,7 @@
     </row>
     <row r="4" spans="1:72">
       <c r="A4">
-        <v>2394588</v>
+        <v>2406750</v>
       </c>
       <c r="C4" t="s">
         <v>78</v>
@@ -2915,11 +2972,68 @@
       <c r="G4" t="s">
         <v>79</v>
       </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
       <c r="AC4">
         <v>1</v>
       </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
       <c r="AV4">
         <v>0</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="BA4">
+        <v>0</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
+      </c>
+      <c r="BD4">
+        <v>0</v>
+      </c>
+      <c r="BE4">
+        <v>0</v>
+      </c>
+      <c r="BF4">
+        <v>0</v>
+      </c>
+      <c r="BG4">
+        <v>0</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>80</v>
       </c>
       <c r="BM4">
         <v>0</v>
@@ -2939,25 +3053,76 @@
     </row>
     <row r="5" spans="1:72">
       <c r="A5">
-        <v>2394587</v>
+        <v>2406749</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
         <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
       </c>
       <c r="AC5">
         <v>1</v>
       </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
       <c r="AV5">
         <v>0</v>
       </c>
-      <c r="BH5" t="s">
-        <v>82</v>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="BA5">
+        <v>0</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+      <c r="BC5">
+        <v>0</v>
+      </c>
+      <c r="BD5">
+        <v>0</v>
+      </c>
+      <c r="BE5">
+        <v>0</v>
+      </c>
+      <c r="BF5">
+        <v>0</v>
+      </c>
+      <c r="BG5">
+        <v>0</v>
       </c>
       <c r="BM5">
         <v>0</v>
@@ -2977,7 +3142,7 @@
     </row>
     <row r="6" spans="1:72">
       <c r="A6">
-        <v>2394586</v>
+        <v>2406748</v>
       </c>
       <c r="C6" t="s">
         <v>83</v>
@@ -2988,11 +3153,68 @@
       <c r="G6" t="s">
         <v>84</v>
       </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
       <c r="AC6">
         <v>1</v>
       </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
       <c r="AV6">
         <v>0</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
+      <c r="BC6">
+        <v>0</v>
+      </c>
+      <c r="BD6">
+        <v>0</v>
+      </c>
+      <c r="BE6">
+        <v>0</v>
+      </c>
+      <c r="BF6">
+        <v>0</v>
+      </c>
+      <c r="BG6">
+        <v>0</v>
+      </c>
+      <c r="BH6" t="s">
+        <v>85</v>
       </c>
       <c r="BM6">
         <v>0</v>
@@ -3012,25 +3234,79 @@
     </row>
     <row r="7" spans="1:72">
       <c r="A7">
-        <v>2394585</v>
+        <v>2406747</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
         <v>73</v>
       </c>
       <c r="G7" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
       </c>
       <c r="AC7">
         <v>1</v>
       </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
       <c r="AV7">
         <v>0</v>
       </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="BA7">
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <v>0</v>
+      </c>
+      <c r="BC7">
+        <v>0</v>
+      </c>
+      <c r="BD7">
+        <v>0</v>
+      </c>
+      <c r="BE7">
+        <v>0</v>
+      </c>
+      <c r="BF7">
+        <v>0</v>
+      </c>
+      <c r="BG7">
+        <v>0</v>
+      </c>
       <c r="BH7" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="BM7">
         <v>0</v>
@@ -3050,25 +3326,76 @@
     </row>
     <row r="8" spans="1:72">
       <c r="A8">
-        <v>2394584</v>
+        <v>2406746</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
         <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
       </c>
       <c r="AC8">
         <v>1</v>
       </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
       <c r="AV8">
         <v>0</v>
       </c>
-      <c r="BH8" t="s">
-        <v>89</v>
+      <c r="AX8">
+        <v>0</v>
+      </c>
+      <c r="AY8">
+        <v>0</v>
+      </c>
+      <c r="BA8">
+        <v>0</v>
+      </c>
+      <c r="BB8">
+        <v>0</v>
+      </c>
+      <c r="BC8">
+        <v>0</v>
+      </c>
+      <c r="BD8">
+        <v>0</v>
+      </c>
+      <c r="BE8">
+        <v>0</v>
+      </c>
+      <c r="BF8">
+        <v>0</v>
+      </c>
+      <c r="BG8">
+        <v>0</v>
       </c>
       <c r="BM8">
         <v>0</v>
@@ -3088,22 +3415,79 @@
     </row>
     <row r="9" spans="1:72">
       <c r="A9">
-        <v>2394583</v>
+        <v>2406745</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
         <v>73</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
       </c>
       <c r="AC9">
         <v>1</v>
       </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
       <c r="AV9">
         <v>0</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
+      </c>
+      <c r="BA9">
+        <v>0</v>
+      </c>
+      <c r="BB9">
+        <v>0</v>
+      </c>
+      <c r="BC9">
+        <v>0</v>
+      </c>
+      <c r="BD9">
+        <v>0</v>
+      </c>
+      <c r="BE9">
+        <v>0</v>
+      </c>
+      <c r="BF9">
+        <v>0</v>
+      </c>
+      <c r="BG9">
+        <v>0</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>88</v>
       </c>
       <c r="BM9">
         <v>0</v>
@@ -3123,25 +3507,76 @@
     </row>
     <row r="10" spans="1:72">
       <c r="A10">
-        <v>2394582</v>
+        <v>2406744</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
         <v>73</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
       </c>
       <c r="AC10">
         <v>1</v>
       </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
       <c r="AV10">
         <v>0</v>
       </c>
-      <c r="BH10" t="s">
-        <v>94</v>
+      <c r="AX10">
+        <v>0</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+      <c r="BA10">
+        <v>0</v>
+      </c>
+      <c r="BB10">
+        <v>0</v>
+      </c>
+      <c r="BC10">
+        <v>0</v>
+      </c>
+      <c r="BD10">
+        <v>0</v>
+      </c>
+      <c r="BE10">
+        <v>0</v>
+      </c>
+      <c r="BF10">
+        <v>0</v>
+      </c>
+      <c r="BG10">
+        <v>0</v>
       </c>
       <c r="BM10">
         <v>0</v>
@@ -3161,7 +3596,7 @@
     </row>
     <row r="11" spans="1:72">
       <c r="A11">
-        <v>2394029</v>
+        <v>2406743</v>
       </c>
       <c r="C11" t="s">
         <v>95</v>
@@ -3434,7 +3869,7 @@
     </row>
     <row r="14" spans="1:72">
       <c r="A14">
-        <v>2394590</v>
+        <v>2406752</v>
       </c>
       <c r="C14" t="s">
         <v>103</v>
@@ -3445,10 +3880,64 @@
       <c r="G14" t="s">
         <v>104</v>
       </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
       <c r="AC14">
         <v>1</v>
       </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AS14">
+        <v>0</v>
+      </c>
       <c r="AV14">
+        <v>0</v>
+      </c>
+      <c r="AX14">
+        <v>0</v>
+      </c>
+      <c r="AY14">
+        <v>0</v>
+      </c>
+      <c r="BA14">
+        <v>0</v>
+      </c>
+      <c r="BB14">
+        <v>0</v>
+      </c>
+      <c r="BC14">
+        <v>0</v>
+      </c>
+      <c r="BD14">
+        <v>0</v>
+      </c>
+      <c r="BE14">
+        <v>0</v>
+      </c>
+      <c r="BF14">
+        <v>0</v>
+      </c>
+      <c r="BG14">
         <v>0</v>
       </c>
       <c r="BM14">
@@ -3541,7 +4030,7 @@
         <v>0</v>
       </c>
       <c r="BH15" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="BM15">
         <v>0</v>
@@ -3633,7 +4122,7 @@
         <v>0</v>
       </c>
       <c r="BH16" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="BM16">
         <v>0</v>
@@ -4475,7 +4964,7 @@
     </row>
     <row r="26" spans="1:72">
       <c r="A26">
-        <v>2394617</v>
+        <v>2406764</v>
       </c>
       <c r="C26" t="s">
         <v>130</v>
@@ -4486,14 +4975,68 @@
       <c r="G26" t="s">
         <v>131</v>
       </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
       <c r="AC26">
         <v>1</v>
       </c>
+      <c r="AI26">
+        <v>0</v>
+      </c>
+      <c r="AJ26">
+        <v>0</v>
+      </c>
+      <c r="AK26">
+        <v>0</v>
+      </c>
+      <c r="AL26">
+        <v>0</v>
+      </c>
+      <c r="AM26">
+        <v>0</v>
+      </c>
+      <c r="AS26">
+        <v>0</v>
+      </c>
       <c r="AV26">
         <v>0</v>
       </c>
+      <c r="AX26">
+        <v>0</v>
+      </c>
+      <c r="AY26">
+        <v>0</v>
+      </c>
+      <c r="BA26">
+        <v>0</v>
+      </c>
+      <c r="BB26">
+        <v>0</v>
+      </c>
+      <c r="BC26">
+        <v>0</v>
+      </c>
+      <c r="BD26">
+        <v>0</v>
+      </c>
+      <c r="BE26">
+        <v>0</v>
+      </c>
+      <c r="BF26">
+        <v>0</v>
+      </c>
+      <c r="BG26">
+        <v>0</v>
+      </c>
       <c r="BH26" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
       <c r="BM26">
         <v>0</v>
@@ -4513,21 +5056,75 @@
     </row>
     <row r="27" spans="1:72">
       <c r="A27">
-        <v>2394628</v>
+        <v>2406775</v>
       </c>
       <c r="C27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D27" t="s">
         <v>73</v>
       </c>
       <c r="G27" t="s">
-        <v>133</v>
+        <v>134</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
       </c>
       <c r="AC27">
         <v>1</v>
       </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
+      </c>
+      <c r="AM27">
+        <v>0</v>
+      </c>
+      <c r="AS27">
+        <v>0</v>
+      </c>
       <c r="AV27">
+        <v>0</v>
+      </c>
+      <c r="AX27">
+        <v>0</v>
+      </c>
+      <c r="AY27">
+        <v>0</v>
+      </c>
+      <c r="BA27">
+        <v>0</v>
+      </c>
+      <c r="BB27">
+        <v>0</v>
+      </c>
+      <c r="BC27">
+        <v>0</v>
+      </c>
+      <c r="BD27">
+        <v>0</v>
+      </c>
+      <c r="BE27">
+        <v>0</v>
+      </c>
+      <c r="BF27">
+        <v>0</v>
+      </c>
+      <c r="BG27">
         <v>0</v>
       </c>
       <c r="BM27">
@@ -4548,21 +5145,75 @@
     </row>
     <row r="28" spans="1:72">
       <c r="A28">
-        <v>2394627</v>
+        <v>2406774</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D28" t="s">
         <v>73</v>
       </c>
       <c r="G28" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
       </c>
       <c r="AC28">
         <v>1</v>
       </c>
+      <c r="AI28">
+        <v>0</v>
+      </c>
+      <c r="AJ28">
+        <v>0</v>
+      </c>
+      <c r="AK28">
+        <v>0</v>
+      </c>
+      <c r="AL28">
+        <v>0</v>
+      </c>
+      <c r="AM28">
+        <v>0</v>
+      </c>
+      <c r="AS28">
+        <v>0</v>
+      </c>
       <c r="AV28">
+        <v>0</v>
+      </c>
+      <c r="AX28">
+        <v>0</v>
+      </c>
+      <c r="AY28">
+        <v>0</v>
+      </c>
+      <c r="BA28">
+        <v>0</v>
+      </c>
+      <c r="BB28">
+        <v>0</v>
+      </c>
+      <c r="BC28">
+        <v>0</v>
+      </c>
+      <c r="BD28">
+        <v>0</v>
+      </c>
+      <c r="BE28">
+        <v>0</v>
+      </c>
+      <c r="BF28">
+        <v>0</v>
+      </c>
+      <c r="BG28">
         <v>0</v>
       </c>
       <c r="BM28">
@@ -4583,22 +5234,79 @@
     </row>
     <row r="29" spans="1:72">
       <c r="A29">
-        <v>2394626</v>
+        <v>2406773</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D29" t="s">
         <v>73</v>
       </c>
       <c r="G29" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
       </c>
       <c r="AC29">
         <v>1</v>
       </c>
+      <c r="AI29">
+        <v>0</v>
+      </c>
+      <c r="AJ29">
+        <v>0</v>
+      </c>
+      <c r="AK29">
+        <v>0</v>
+      </c>
+      <c r="AL29">
+        <v>0</v>
+      </c>
+      <c r="AM29">
+        <v>0</v>
+      </c>
+      <c r="AS29">
+        <v>0</v>
+      </c>
       <c r="AV29">
         <v>0</v>
+      </c>
+      <c r="AX29">
+        <v>0</v>
+      </c>
+      <c r="AY29">
+        <v>0</v>
+      </c>
+      <c r="BA29">
+        <v>0</v>
+      </c>
+      <c r="BB29">
+        <v>0</v>
+      </c>
+      <c r="BC29">
+        <v>0</v>
+      </c>
+      <c r="BD29">
+        <v>0</v>
+      </c>
+      <c r="BE29">
+        <v>0</v>
+      </c>
+      <c r="BF29">
+        <v>0</v>
+      </c>
+      <c r="BG29">
+        <v>0</v>
+      </c>
+      <c r="BH29" t="s">
+        <v>97</v>
       </c>
       <c r="BM29">
         <v>0</v>
@@ -4618,22 +5326,79 @@
     </row>
     <row r="30" spans="1:72">
       <c r="A30">
-        <v>2394625</v>
+        <v>2406772</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D30" t="s">
         <v>73</v>
       </c>
       <c r="G30" t="s">
-        <v>139</v>
+        <v>140</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
       </c>
       <c r="AC30">
         <v>1</v>
       </c>
+      <c r="AI30">
+        <v>0</v>
+      </c>
+      <c r="AJ30">
+        <v>0</v>
+      </c>
+      <c r="AK30">
+        <v>0</v>
+      </c>
+      <c r="AL30">
+        <v>0</v>
+      </c>
+      <c r="AM30">
+        <v>0</v>
+      </c>
+      <c r="AS30">
+        <v>0</v>
+      </c>
       <c r="AV30">
         <v>0</v>
+      </c>
+      <c r="AX30">
+        <v>0</v>
+      </c>
+      <c r="AY30">
+        <v>0</v>
+      </c>
+      <c r="BA30">
+        <v>0</v>
+      </c>
+      <c r="BB30">
+        <v>0</v>
+      </c>
+      <c r="BC30">
+        <v>0</v>
+      </c>
+      <c r="BD30">
+        <v>0</v>
+      </c>
+      <c r="BE30">
+        <v>0</v>
+      </c>
+      <c r="BF30">
+        <v>0</v>
+      </c>
+      <c r="BG30">
+        <v>0</v>
+      </c>
+      <c r="BH30" t="s">
+        <v>80</v>
       </c>
       <c r="BM30">
         <v>0</v>
@@ -4653,22 +5418,79 @@
     </row>
     <row r="31" spans="1:72">
       <c r="A31">
-        <v>2394624</v>
+        <v>2406771</v>
       </c>
       <c r="C31" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D31" t="s">
         <v>73</v>
       </c>
       <c r="G31" t="s">
-        <v>141</v>
+        <v>142</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>0</v>
       </c>
       <c r="AC31">
         <v>1</v>
       </c>
+      <c r="AI31">
+        <v>0</v>
+      </c>
+      <c r="AJ31">
+        <v>0</v>
+      </c>
+      <c r="AK31">
+        <v>0</v>
+      </c>
+      <c r="AL31">
+        <v>0</v>
+      </c>
+      <c r="AM31">
+        <v>0</v>
+      </c>
+      <c r="AS31">
+        <v>0</v>
+      </c>
       <c r="AV31">
         <v>0</v>
+      </c>
+      <c r="AX31">
+        <v>0</v>
+      </c>
+      <c r="AY31">
+        <v>0</v>
+      </c>
+      <c r="BA31">
+        <v>0</v>
+      </c>
+      <c r="BB31">
+        <v>0</v>
+      </c>
+      <c r="BC31">
+        <v>0</v>
+      </c>
+      <c r="BD31">
+        <v>0</v>
+      </c>
+      <c r="BE31">
+        <v>0</v>
+      </c>
+      <c r="BF31">
+        <v>0</v>
+      </c>
+      <c r="BG31">
+        <v>0</v>
+      </c>
+      <c r="BH31" t="s">
+        <v>132</v>
       </c>
       <c r="BM31">
         <v>0</v>
@@ -4688,22 +5510,79 @@
     </row>
     <row r="32" spans="1:72">
       <c r="A32">
-        <v>2394623</v>
+        <v>2406770</v>
       </c>
       <c r="C32" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D32" t="s">
         <v>73</v>
       </c>
       <c r="G32" t="s">
-        <v>143</v>
+        <v>144</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
       </c>
       <c r="AC32">
         <v>1</v>
       </c>
+      <c r="AI32">
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <v>0</v>
+      </c>
+      <c r="AK32">
+        <v>0</v>
+      </c>
+      <c r="AL32">
+        <v>0</v>
+      </c>
+      <c r="AM32">
+        <v>0</v>
+      </c>
+      <c r="AS32">
+        <v>0</v>
+      </c>
       <c r="AV32">
         <v>0</v>
+      </c>
+      <c r="AX32">
+        <v>0</v>
+      </c>
+      <c r="AY32">
+        <v>0</v>
+      </c>
+      <c r="BA32">
+        <v>0</v>
+      </c>
+      <c r="BB32">
+        <v>0</v>
+      </c>
+      <c r="BC32">
+        <v>0</v>
+      </c>
+      <c r="BD32">
+        <v>0</v>
+      </c>
+      <c r="BE32">
+        <v>0</v>
+      </c>
+      <c r="BF32">
+        <v>0</v>
+      </c>
+      <c r="BG32">
+        <v>0</v>
+      </c>
+      <c r="BH32" t="s">
+        <v>132</v>
       </c>
       <c r="BM32">
         <v>0</v>
@@ -4723,22 +5602,79 @@
     </row>
     <row r="33" spans="1:72">
       <c r="A33">
-        <v>2394622</v>
+        <v>2406769</v>
       </c>
       <c r="C33" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D33" t="s">
         <v>73</v>
       </c>
       <c r="G33" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
       </c>
       <c r="AC33">
         <v>1</v>
       </c>
+      <c r="AI33">
+        <v>0</v>
+      </c>
+      <c r="AJ33">
+        <v>0</v>
+      </c>
+      <c r="AK33">
+        <v>0</v>
+      </c>
+      <c r="AL33">
+        <v>0</v>
+      </c>
+      <c r="AM33">
+        <v>0</v>
+      </c>
+      <c r="AS33">
+        <v>0</v>
+      </c>
       <c r="AV33">
         <v>0</v>
+      </c>
+      <c r="AX33">
+        <v>0</v>
+      </c>
+      <c r="AY33">
+        <v>0</v>
+      </c>
+      <c r="BA33">
+        <v>0</v>
+      </c>
+      <c r="BB33">
+        <v>0</v>
+      </c>
+      <c r="BC33">
+        <v>0</v>
+      </c>
+      <c r="BD33">
+        <v>0</v>
+      </c>
+      <c r="BE33">
+        <v>0</v>
+      </c>
+      <c r="BF33">
+        <v>0</v>
+      </c>
+      <c r="BG33">
+        <v>0</v>
+      </c>
+      <c r="BH33" t="s">
+        <v>132</v>
       </c>
       <c r="BM33">
         <v>0</v>
@@ -4758,25 +5694,79 @@
     </row>
     <row r="34" spans="1:72">
       <c r="A34">
-        <v>2394621</v>
+        <v>2406768</v>
       </c>
       <c r="C34" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D34" t="s">
         <v>73</v>
       </c>
       <c r="G34" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
       </c>
       <c r="AC34">
         <v>1</v>
       </c>
+      <c r="AI34">
+        <v>0</v>
+      </c>
+      <c r="AJ34">
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <v>0</v>
+      </c>
+      <c r="AL34">
+        <v>0</v>
+      </c>
+      <c r="AM34">
+        <v>0</v>
+      </c>
+      <c r="AS34">
+        <v>0</v>
+      </c>
       <c r="AV34">
         <v>0</v>
       </c>
+      <c r="AX34">
+        <v>0</v>
+      </c>
+      <c r="AY34">
+        <v>0</v>
+      </c>
+      <c r="BA34">
+        <v>0</v>
+      </c>
+      <c r="BB34">
+        <v>0</v>
+      </c>
+      <c r="BC34">
+        <v>0</v>
+      </c>
+      <c r="BD34">
+        <v>0</v>
+      </c>
+      <c r="BE34">
+        <v>0</v>
+      </c>
+      <c r="BF34">
+        <v>0</v>
+      </c>
+      <c r="BG34">
+        <v>0</v>
+      </c>
       <c r="BH34" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="BM34">
         <v>0</v>
@@ -4796,7 +5786,7 @@
     </row>
     <row r="35" spans="1:72">
       <c r="A35">
-        <v>2394620</v>
+        <v>2406767</v>
       </c>
       <c r="C35" t="s">
         <v>149</v>
@@ -4807,14 +5797,65 @@
       <c r="G35" t="s">
         <v>150</v>
       </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>0</v>
+      </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
       <c r="AC35">
         <v>1</v>
       </c>
+      <c r="AI35">
+        <v>0</v>
+      </c>
+      <c r="AJ35">
+        <v>0</v>
+      </c>
+      <c r="AK35">
+        <v>0</v>
+      </c>
+      <c r="AL35">
+        <v>0</v>
+      </c>
+      <c r="AM35">
+        <v>0</v>
+      </c>
+      <c r="AS35">
+        <v>0</v>
+      </c>
       <c r="AV35">
         <v>0</v>
       </c>
-      <c r="BH35" t="s">
-        <v>148</v>
+      <c r="AX35">
+        <v>0</v>
+      </c>
+      <c r="AY35">
+        <v>0</v>
+      </c>
+      <c r="BA35">
+        <v>0</v>
+      </c>
+      <c r="BB35">
+        <v>0</v>
+      </c>
+      <c r="BC35">
+        <v>0</v>
+      </c>
+      <c r="BD35">
+        <v>0</v>
+      </c>
+      <c r="BE35">
+        <v>0</v>
+      </c>
+      <c r="BF35">
+        <v>0</v>
+      </c>
+      <c r="BG35">
+        <v>0</v>
       </c>
       <c r="BM35">
         <v>0</v>
@@ -4834,7 +5875,7 @@
     </row>
     <row r="36" spans="1:72">
       <c r="A36">
-        <v>2394619</v>
+        <v>2406766</v>
       </c>
       <c r="C36" t="s">
         <v>151</v>
@@ -4845,14 +5886,68 @@
       <c r="G36" t="s">
         <v>152</v>
       </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>0</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
       <c r="AC36">
         <v>1</v>
       </c>
+      <c r="AI36">
+        <v>0</v>
+      </c>
+      <c r="AJ36">
+        <v>0</v>
+      </c>
+      <c r="AK36">
+        <v>0</v>
+      </c>
+      <c r="AL36">
+        <v>0</v>
+      </c>
+      <c r="AM36">
+        <v>0</v>
+      </c>
+      <c r="AS36">
+        <v>0</v>
+      </c>
       <c r="AV36">
         <v>0</v>
       </c>
+      <c r="AX36">
+        <v>0</v>
+      </c>
+      <c r="AY36">
+        <v>0</v>
+      </c>
+      <c r="BA36">
+        <v>0</v>
+      </c>
+      <c r="BB36">
+        <v>0</v>
+      </c>
+      <c r="BC36">
+        <v>0</v>
+      </c>
+      <c r="BD36">
+        <v>0</v>
+      </c>
+      <c r="BE36">
+        <v>0</v>
+      </c>
+      <c r="BF36">
+        <v>0</v>
+      </c>
+      <c r="BG36">
+        <v>0</v>
+      </c>
       <c r="BH36" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="BM36">
         <v>0</v>
@@ -4872,7 +5967,7 @@
     </row>
     <row r="37" spans="1:72">
       <c r="A37">
-        <v>2394618</v>
+        <v>2406765</v>
       </c>
       <c r="C37" t="s">
         <v>153</v>
@@ -4883,14 +5978,65 @@
       <c r="G37" t="s">
         <v>154</v>
       </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="Y37">
+        <v>0</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
       <c r="AC37">
         <v>1</v>
       </c>
+      <c r="AI37">
+        <v>0</v>
+      </c>
+      <c r="AJ37">
+        <v>0</v>
+      </c>
+      <c r="AK37">
+        <v>0</v>
+      </c>
+      <c r="AL37">
+        <v>0</v>
+      </c>
+      <c r="AM37">
+        <v>0</v>
+      </c>
+      <c r="AS37">
+        <v>0</v>
+      </c>
       <c r="AV37">
         <v>0</v>
       </c>
-      <c r="BH37" t="s">
-        <v>148</v>
+      <c r="AX37">
+        <v>0</v>
+      </c>
+      <c r="AY37">
+        <v>0</v>
+      </c>
+      <c r="BA37">
+        <v>0</v>
+      </c>
+      <c r="BB37">
+        <v>0</v>
+      </c>
+      <c r="BC37">
+        <v>0</v>
+      </c>
+      <c r="BD37">
+        <v>0</v>
+      </c>
+      <c r="BE37">
+        <v>0</v>
+      </c>
+      <c r="BF37">
+        <v>0</v>
+      </c>
+      <c r="BG37">
+        <v>0</v>
       </c>
       <c r="BM37">
         <v>0</v>
@@ -5002,7 +6148,7 @@
     </row>
     <row r="39" spans="1:72">
       <c r="A39">
-        <v>2394616</v>
+        <v>2406763</v>
       </c>
       <c r="C39" t="s">
         <v>158</v>
@@ -5013,11 +6159,68 @@
       <c r="G39" t="s">
         <v>159</v>
       </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="Y39">
+        <v>0</v>
+      </c>
+      <c r="Z39">
+        <v>0</v>
+      </c>
       <c r="AC39">
         <v>1</v>
       </c>
+      <c r="AI39">
+        <v>0</v>
+      </c>
+      <c r="AJ39">
+        <v>0</v>
+      </c>
+      <c r="AK39">
+        <v>0</v>
+      </c>
+      <c r="AL39">
+        <v>0</v>
+      </c>
+      <c r="AM39">
+        <v>0</v>
+      </c>
+      <c r="AS39">
+        <v>0</v>
+      </c>
       <c r="AV39">
         <v>0</v>
+      </c>
+      <c r="AX39">
+        <v>0</v>
+      </c>
+      <c r="AY39">
+        <v>0</v>
+      </c>
+      <c r="BA39">
+        <v>0</v>
+      </c>
+      <c r="BB39">
+        <v>0</v>
+      </c>
+      <c r="BC39">
+        <v>0</v>
+      </c>
+      <c r="BD39">
+        <v>0</v>
+      </c>
+      <c r="BE39">
+        <v>0</v>
+      </c>
+      <c r="BF39">
+        <v>0</v>
+      </c>
+      <c r="BG39">
+        <v>0</v>
+      </c>
+      <c r="BH39" t="s">
+        <v>132</v>
       </c>
       <c r="BM39">
         <v>0</v>
@@ -5037,7 +6240,7 @@
     </row>
     <row r="40" spans="1:72">
       <c r="A40">
-        <v>2394615</v>
+        <v>2406762</v>
       </c>
       <c r="C40" t="s">
         <v>160</v>
@@ -5048,14 +6251,68 @@
       <c r="G40" t="s">
         <v>161</v>
       </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="Y40">
+        <v>0</v>
+      </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
       <c r="AC40">
         <v>1</v>
       </c>
+      <c r="AI40">
+        <v>0</v>
+      </c>
+      <c r="AJ40">
+        <v>0</v>
+      </c>
+      <c r="AK40">
+        <v>0</v>
+      </c>
+      <c r="AL40">
+        <v>0</v>
+      </c>
+      <c r="AM40">
+        <v>0</v>
+      </c>
+      <c r="AS40">
+        <v>0</v>
+      </c>
       <c r="AV40">
         <v>0</v>
       </c>
+      <c r="AX40">
+        <v>0</v>
+      </c>
+      <c r="AY40">
+        <v>0</v>
+      </c>
+      <c r="BA40">
+        <v>0</v>
+      </c>
+      <c r="BB40">
+        <v>0</v>
+      </c>
+      <c r="BC40">
+        <v>0</v>
+      </c>
+      <c r="BD40">
+        <v>0</v>
+      </c>
+      <c r="BE40">
+        <v>0</v>
+      </c>
+      <c r="BF40">
+        <v>0</v>
+      </c>
+      <c r="BG40">
+        <v>0</v>
+      </c>
       <c r="BH40" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="BM40">
         <v>0</v>
@@ -5075,7 +6332,7 @@
     </row>
     <row r="41" spans="1:72">
       <c r="A41">
-        <v>2394614</v>
+        <v>2406761</v>
       </c>
       <c r="C41" t="s">
         <v>162</v>
@@ -5086,11 +6343,68 @@
       <c r="G41" t="s">
         <v>163</v>
       </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="Y41">
+        <v>0</v>
+      </c>
+      <c r="Z41">
+        <v>0</v>
+      </c>
       <c r="AC41">
         <v>1</v>
       </c>
+      <c r="AI41">
+        <v>0</v>
+      </c>
+      <c r="AJ41">
+        <v>0</v>
+      </c>
+      <c r="AK41">
+        <v>0</v>
+      </c>
+      <c r="AL41">
+        <v>0</v>
+      </c>
+      <c r="AM41">
+        <v>0</v>
+      </c>
+      <c r="AS41">
+        <v>0</v>
+      </c>
       <c r="AV41">
         <v>0</v>
+      </c>
+      <c r="AX41">
+        <v>0</v>
+      </c>
+      <c r="AY41">
+        <v>0</v>
+      </c>
+      <c r="BA41">
+        <v>0</v>
+      </c>
+      <c r="BB41">
+        <v>0</v>
+      </c>
+      <c r="BC41">
+        <v>0</v>
+      </c>
+      <c r="BD41">
+        <v>0</v>
+      </c>
+      <c r="BE41">
+        <v>0</v>
+      </c>
+      <c r="BF41">
+        <v>0</v>
+      </c>
+      <c r="BG41">
+        <v>0</v>
+      </c>
+      <c r="BH41" t="s">
+        <v>132</v>
       </c>
       <c r="BM41">
         <v>0</v>
@@ -5110,7 +6424,7 @@
     </row>
     <row r="42" spans="1:72">
       <c r="A42">
-        <v>2394613</v>
+        <v>2406760</v>
       </c>
       <c r="C42" t="s">
         <v>164</v>
@@ -5121,14 +6435,65 @@
       <c r="G42" t="s">
         <v>165</v>
       </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="Y42">
+        <v>0</v>
+      </c>
+      <c r="Z42">
+        <v>0</v>
+      </c>
       <c r="AC42">
         <v>1</v>
       </c>
+      <c r="AI42">
+        <v>0</v>
+      </c>
+      <c r="AJ42">
+        <v>0</v>
+      </c>
+      <c r="AK42">
+        <v>0</v>
+      </c>
+      <c r="AL42">
+        <v>0</v>
+      </c>
+      <c r="AM42">
+        <v>0</v>
+      </c>
+      <c r="AS42">
+        <v>0</v>
+      </c>
       <c r="AV42">
         <v>0</v>
       </c>
-      <c r="BH42" t="s">
-        <v>148</v>
+      <c r="AX42">
+        <v>0</v>
+      </c>
+      <c r="AY42">
+        <v>0</v>
+      </c>
+      <c r="BA42">
+        <v>0</v>
+      </c>
+      <c r="BB42">
+        <v>0</v>
+      </c>
+      <c r="BC42">
+        <v>0</v>
+      </c>
+      <c r="BD42">
+        <v>0</v>
+      </c>
+      <c r="BE42">
+        <v>0</v>
+      </c>
+      <c r="BF42">
+        <v>0</v>
+      </c>
+      <c r="BG42">
+        <v>0</v>
       </c>
       <c r="BM42">
         <v>0</v>
@@ -5148,7 +6513,7 @@
     </row>
     <row r="43" spans="1:72">
       <c r="A43">
-        <v>2394612</v>
+        <v>2406759</v>
       </c>
       <c r="C43" t="s">
         <v>166</v>
@@ -5159,14 +6524,65 @@
       <c r="G43" t="s">
         <v>167</v>
       </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="Y43">
+        <v>0</v>
+      </c>
+      <c r="Z43">
+        <v>0</v>
+      </c>
       <c r="AC43">
         <v>1</v>
       </c>
+      <c r="AI43">
+        <v>0</v>
+      </c>
+      <c r="AJ43">
+        <v>0</v>
+      </c>
+      <c r="AK43">
+        <v>0</v>
+      </c>
+      <c r="AL43">
+        <v>0</v>
+      </c>
+      <c r="AM43">
+        <v>0</v>
+      </c>
+      <c r="AS43">
+        <v>0</v>
+      </c>
       <c r="AV43">
         <v>0</v>
       </c>
-      <c r="BH43" t="s">
-        <v>148</v>
+      <c r="AX43">
+        <v>0</v>
+      </c>
+      <c r="AY43">
+        <v>0</v>
+      </c>
+      <c r="BA43">
+        <v>0</v>
+      </c>
+      <c r="BB43">
+        <v>0</v>
+      </c>
+      <c r="BC43">
+        <v>0</v>
+      </c>
+      <c r="BD43">
+        <v>0</v>
+      </c>
+      <c r="BE43">
+        <v>0</v>
+      </c>
+      <c r="BF43">
+        <v>0</v>
+      </c>
+      <c r="BG43">
+        <v>0</v>
       </c>
       <c r="BM43">
         <v>0</v>
@@ -5186,7 +6602,7 @@
     </row>
     <row r="44" spans="1:72">
       <c r="A44">
-        <v>2394611</v>
+        <v>2406758</v>
       </c>
       <c r="C44" t="s">
         <v>168</v>
@@ -5197,14 +6613,65 @@
       <c r="G44" t="s">
         <v>169</v>
       </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="Y44">
+        <v>0</v>
+      </c>
+      <c r="Z44">
+        <v>0</v>
+      </c>
       <c r="AC44">
         <v>1</v>
       </c>
+      <c r="AI44">
+        <v>0</v>
+      </c>
+      <c r="AJ44">
+        <v>0</v>
+      </c>
+      <c r="AK44">
+        <v>0</v>
+      </c>
+      <c r="AL44">
+        <v>0</v>
+      </c>
+      <c r="AM44">
+        <v>0</v>
+      </c>
+      <c r="AS44">
+        <v>0</v>
+      </c>
       <c r="AV44">
         <v>0</v>
       </c>
-      <c r="BH44" t="s">
-        <v>148</v>
+      <c r="AX44">
+        <v>0</v>
+      </c>
+      <c r="AY44">
+        <v>0</v>
+      </c>
+      <c r="BA44">
+        <v>0</v>
+      </c>
+      <c r="BB44">
+        <v>0</v>
+      </c>
+      <c r="BC44">
+        <v>0</v>
+      </c>
+      <c r="BD44">
+        <v>0</v>
+      </c>
+      <c r="BE44">
+        <v>0</v>
+      </c>
+      <c r="BF44">
+        <v>0</v>
+      </c>
+      <c r="BG44">
+        <v>0</v>
       </c>
       <c r="BM44">
         <v>0</v>
@@ -5224,7 +6691,7 @@
     </row>
     <row r="45" spans="1:72">
       <c r="A45">
-        <v>2394595</v>
+        <v>2406757</v>
       </c>
       <c r="C45" t="s">
         <v>170</v>
@@ -5235,14 +6702,65 @@
       <c r="G45" t="s">
         <v>171</v>
       </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="Y45">
+        <v>0</v>
+      </c>
+      <c r="Z45">
+        <v>0</v>
+      </c>
       <c r="AC45">
         <v>1</v>
       </c>
+      <c r="AI45">
+        <v>0</v>
+      </c>
+      <c r="AJ45">
+        <v>0</v>
+      </c>
+      <c r="AK45">
+        <v>0</v>
+      </c>
+      <c r="AL45">
+        <v>0</v>
+      </c>
+      <c r="AM45">
+        <v>0</v>
+      </c>
+      <c r="AS45">
+        <v>0</v>
+      </c>
       <c r="AV45">
         <v>0</v>
       </c>
-      <c r="BH45" t="s">
-        <v>148</v>
+      <c r="AX45">
+        <v>0</v>
+      </c>
+      <c r="AY45">
+        <v>0</v>
+      </c>
+      <c r="BA45">
+        <v>0</v>
+      </c>
+      <c r="BB45">
+        <v>0</v>
+      </c>
+      <c r="BC45">
+        <v>0</v>
+      </c>
+      <c r="BD45">
+        <v>0</v>
+      </c>
+      <c r="BE45">
+        <v>0</v>
+      </c>
+      <c r="BF45">
+        <v>0</v>
+      </c>
+      <c r="BG45">
+        <v>0</v>
       </c>
       <c r="BM45">
         <v>0</v>
@@ -5262,7 +6780,7 @@
     </row>
     <row r="46" spans="1:72">
       <c r="A46">
-        <v>2394594</v>
+        <v>2406756</v>
       </c>
       <c r="C46" t="s">
         <v>172</v>
@@ -5273,14 +6791,65 @@
       <c r="G46" t="s">
         <v>173</v>
       </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="Y46">
+        <v>0</v>
+      </c>
+      <c r="Z46">
+        <v>0</v>
+      </c>
       <c r="AC46">
         <v>1</v>
       </c>
+      <c r="AI46">
+        <v>0</v>
+      </c>
+      <c r="AJ46">
+        <v>0</v>
+      </c>
+      <c r="AK46">
+        <v>0</v>
+      </c>
+      <c r="AL46">
+        <v>0</v>
+      </c>
+      <c r="AM46">
+        <v>0</v>
+      </c>
+      <c r="AS46">
+        <v>0</v>
+      </c>
       <c r="AV46">
         <v>0</v>
       </c>
-      <c r="BH46" t="s">
-        <v>94</v>
+      <c r="AX46">
+        <v>0</v>
+      </c>
+      <c r="AY46">
+        <v>0</v>
+      </c>
+      <c r="BA46">
+        <v>0</v>
+      </c>
+      <c r="BB46">
+        <v>0</v>
+      </c>
+      <c r="BC46">
+        <v>0</v>
+      </c>
+      <c r="BD46">
+        <v>0</v>
+      </c>
+      <c r="BE46">
+        <v>0</v>
+      </c>
+      <c r="BF46">
+        <v>0</v>
+      </c>
+      <c r="BG46">
+        <v>0</v>
       </c>
       <c r="BM46">
         <v>0</v>
@@ -5300,7 +6869,7 @@
     </row>
     <row r="47" spans="1:72">
       <c r="A47">
-        <v>2394593</v>
+        <v>2406755</v>
       </c>
       <c r="C47" t="s">
         <v>174</v>
@@ -5311,14 +6880,65 @@
       <c r="G47" t="s">
         <v>175</v>
       </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="Y47">
+        <v>0</v>
+      </c>
+      <c r="Z47">
+        <v>0</v>
+      </c>
       <c r="AC47">
         <v>1</v>
       </c>
+      <c r="AI47">
+        <v>0</v>
+      </c>
+      <c r="AJ47">
+        <v>0</v>
+      </c>
+      <c r="AK47">
+        <v>0</v>
+      </c>
+      <c r="AL47">
+        <v>0</v>
+      </c>
+      <c r="AM47">
+        <v>0</v>
+      </c>
+      <c r="AS47">
+        <v>0</v>
+      </c>
       <c r="AV47">
         <v>0</v>
       </c>
-      <c r="BH47" t="s">
-        <v>77</v>
+      <c r="AX47">
+        <v>0</v>
+      </c>
+      <c r="AY47">
+        <v>0</v>
+      </c>
+      <c r="BA47">
+        <v>0</v>
+      </c>
+      <c r="BB47">
+        <v>0</v>
+      </c>
+      <c r="BC47">
+        <v>0</v>
+      </c>
+      <c r="BD47">
+        <v>0</v>
+      </c>
+      <c r="BE47">
+        <v>0</v>
+      </c>
+      <c r="BF47">
+        <v>0</v>
+      </c>
+      <c r="BG47">
+        <v>0</v>
       </c>
       <c r="BM47">
         <v>0</v>
@@ -5338,7 +6958,7 @@
     </row>
     <row r="48" spans="1:72">
       <c r="A48">
-        <v>2394592</v>
+        <v>2406754</v>
       </c>
       <c r="C48" t="s">
         <v>176</v>
@@ -5349,10 +6969,64 @@
       <c r="G48" t="s">
         <v>177</v>
       </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="Y48">
+        <v>0</v>
+      </c>
+      <c r="Z48">
+        <v>0</v>
+      </c>
       <c r="AC48">
         <v>1</v>
       </c>
+      <c r="AI48">
+        <v>0</v>
+      </c>
+      <c r="AJ48">
+        <v>0</v>
+      </c>
+      <c r="AK48">
+        <v>0</v>
+      </c>
+      <c r="AL48">
+        <v>0</v>
+      </c>
+      <c r="AM48">
+        <v>0</v>
+      </c>
+      <c r="AS48">
+        <v>0</v>
+      </c>
       <c r="AV48">
+        <v>0</v>
+      </c>
+      <c r="AX48">
+        <v>0</v>
+      </c>
+      <c r="AY48">
+        <v>0</v>
+      </c>
+      <c r="BA48">
+        <v>0</v>
+      </c>
+      <c r="BB48">
+        <v>0</v>
+      </c>
+      <c r="BC48">
+        <v>0</v>
+      </c>
+      <c r="BD48">
+        <v>0</v>
+      </c>
+      <c r="BE48">
+        <v>0</v>
+      </c>
+      <c r="BF48">
+        <v>0</v>
+      </c>
+      <c r="BG48">
         <v>0</v>
       </c>
       <c r="BM48">
@@ -5373,7 +7047,7 @@
     </row>
     <row r="49" spans="1:72">
       <c r="A49">
-        <v>2394591</v>
+        <v>2406753</v>
       </c>
       <c r="C49" t="s">
         <v>178</v>
@@ -5384,11 +7058,68 @@
       <c r="G49" t="s">
         <v>179</v>
       </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <v>0</v>
+      </c>
+      <c r="Z49">
+        <v>0</v>
+      </c>
       <c r="AC49">
         <v>1</v>
       </c>
+      <c r="AI49">
+        <v>0</v>
+      </c>
+      <c r="AJ49">
+        <v>0</v>
+      </c>
+      <c r="AK49">
+        <v>0</v>
+      </c>
+      <c r="AL49">
+        <v>0</v>
+      </c>
+      <c r="AM49">
+        <v>0</v>
+      </c>
+      <c r="AS49">
+        <v>0</v>
+      </c>
       <c r="AV49">
         <v>0</v>
+      </c>
+      <c r="AX49">
+        <v>0</v>
+      </c>
+      <c r="AY49">
+        <v>0</v>
+      </c>
+      <c r="BA49">
+        <v>0</v>
+      </c>
+      <c r="BB49">
+        <v>0</v>
+      </c>
+      <c r="BC49">
+        <v>0</v>
+      </c>
+      <c r="BD49">
+        <v>0</v>
+      </c>
+      <c r="BE49">
+        <v>0</v>
+      </c>
+      <c r="BF49">
+        <v>0</v>
+      </c>
+      <c r="BG49">
+        <v>0</v>
+      </c>
+      <c r="BH49" t="s">
+        <v>97</v>
       </c>
       <c r="BM49">
         <v>0</v>
@@ -5572,7 +7303,7 @@
         <v>0</v>
       </c>
       <c r="BH51" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="BM51">
         <v>0</v>
@@ -6762,7 +8493,7 @@
         <v>0</v>
       </c>
       <c r="BH64" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="BM64">
         <v>0</v>
@@ -7486,7 +9217,7 @@
         <v>0</v>
       </c>
       <c r="BH72" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="BM72">
         <v>0</v>
@@ -8759,7 +10490,7 @@
         <v>0</v>
       </c>
       <c r="BH86" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="BM86">
         <v>0</v>
@@ -23715,7 +25446,7 @@
         <v>0</v>
       </c>
       <c r="BH244" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="BM244">
         <v>0</v>
@@ -23807,7 +25538,7 @@
         <v>0</v>
       </c>
       <c r="BH245" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="BM245">
         <v>0</v>
@@ -23899,7 +25630,7 @@
         <v>0</v>
       </c>
       <c r="BH246" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="BM246">
         <v>0</v>
@@ -24000,7 +25731,7 @@
         <v>0</v>
       </c>
       <c r="BH247" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="BM247">
         <v>0</v>
@@ -24092,7 +25823,7 @@
         <v>0</v>
       </c>
       <c r="BH248" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="BM248">
         <v>0</v>
@@ -24184,7 +25915,7 @@
         <v>0</v>
       </c>
       <c r="BH249" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="BM249">
         <v>0</v>
@@ -24368,7 +26099,7 @@
         <v>0</v>
       </c>
       <c r="BH251" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="BM251">
         <v>0</v>
@@ -24558,7 +26289,7 @@
         <v>0</v>
       </c>
       <c r="BH253" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="BM253">
         <v>0</v>
@@ -24659,7 +26390,7 @@
         <v>0</v>
       </c>
       <c r="BH254" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="BM254">
         <v>0</v>
@@ -24751,7 +26482,7 @@
         <v>0</v>
       </c>
       <c r="BH255" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="BM255">
         <v>0</v>
@@ -24852,7 +26583,7 @@
         <v>0</v>
       </c>
       <c r="BH256" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="BM256">
         <v>0</v>
@@ -24944,7 +26675,7 @@
         <v>0</v>
       </c>
       <c r="BH257" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="BM257">
         <v>0</v>
@@ -25036,7 +26767,7 @@
         <v>0</v>
       </c>
       <c r="BH258" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="BM258">
         <v>0</v>
@@ -26247,7 +27978,7 @@
         <v>0</v>
       </c>
       <c r="BH271" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="BM271">
         <v>0</v>
@@ -26790,7 +28521,7 @@
         <v>0</v>
       </c>
       <c r="BH277" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="BM277">
         <v>0</v>
@@ -26919,6 +28650,9 @@
       <c r="Z279">
         <v>0</v>
       </c>
+      <c r="AA279" t="s">
+        <v>685</v>
+      </c>
       <c r="AC279">
         <v>1</v>
       </c>
@@ -26937,19 +28671,7 @@
       <c r="AM279">
         <v>0</v>
       </c>
-      <c r="AS279">
-        <v>0</v>
-      </c>
       <c r="AV279">
-        <v>0</v>
-      </c>
-      <c r="AX279">
-        <v>0</v>
-      </c>
-      <c r="AY279">
-        <v>0</v>
-      </c>
-      <c r="BA279">
         <v>0</v>
       </c>
       <c r="BB279">
@@ -26991,13 +28713,13 @@
         <v>1170415</v>
       </c>
       <c r="C280" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D280" t="s">
         <v>73</v>
       </c>
       <c r="G280" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="O280">
         <v>0</v>
@@ -27060,7 +28782,7 @@
         <v>0</v>
       </c>
       <c r="BH280" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="BM280">
         <v>0</v>
@@ -27083,13 +28805,13 @@
         <v>1170416</v>
       </c>
       <c r="C281" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="D281" t="s">
         <v>73</v>
       </c>
       <c r="G281" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="O281">
         <v>0</v>
@@ -27175,13 +28897,13 @@
         <v>1170417</v>
       </c>
       <c r="C282" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D282" t="s">
         <v>73</v>
       </c>
       <c r="G282" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="O282">
         <v>0</v>
@@ -27267,13 +28989,13 @@
         <v>1170418</v>
       </c>
       <c r="C283" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="D283" t="s">
         <v>73</v>
       </c>
       <c r="G283" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="O283">
         <v>0</v>
@@ -27336,7 +29058,7 @@
         <v>0</v>
       </c>
       <c r="BH283" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="BM283">
         <v>0</v>
@@ -27359,13 +29081,13 @@
         <v>1170419</v>
       </c>
       <c r="C284" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D284" t="s">
         <v>73</v>
       </c>
       <c r="G284" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="O284">
         <v>0</v>
@@ -27448,13 +29170,13 @@
         <v>1170420</v>
       </c>
       <c r="C285" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="D285" t="s">
         <v>73</v>
       </c>
       <c r="G285" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="O285">
         <v>0</v>
@@ -27517,7 +29239,7 @@
         <v>0</v>
       </c>
       <c r="BH285" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="BM285">
         <v>0</v>
@@ -27540,13 +29262,13 @@
         <v>1170421</v>
       </c>
       <c r="C286" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="D286" t="s">
         <v>73</v>
       </c>
       <c r="G286" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="O286">
         <v>0</v>
@@ -27609,7 +29331,7 @@
         <v>0</v>
       </c>
       <c r="BH286" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="BM286">
         <v>0</v>
@@ -27632,13 +29354,13 @@
         <v>1170422</v>
       </c>
       <c r="C287" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D287" t="s">
         <v>73</v>
       </c>
       <c r="G287" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="O287">
         <v>0</v>
@@ -27701,7 +29423,7 @@
         <v>0</v>
       </c>
       <c r="BH287" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="BM287">
         <v>0</v>
@@ -27724,13 +29446,13 @@
         <v>1170423</v>
       </c>
       <c r="C288" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="D288" t="s">
         <v>73</v>
       </c>
       <c r="G288" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="O288">
         <v>0</v>
@@ -27816,13 +29538,13 @@
         <v>1170424</v>
       </c>
       <c r="C289" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="D289" t="s">
         <v>73</v>
       </c>
       <c r="G289" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="O289">
         <v>0</v>
@@ -27908,13 +29630,13 @@
         <v>1170425</v>
       </c>
       <c r="C290" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="D290" t="s">
         <v>73</v>
       </c>
       <c r="G290" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="O290">
         <v>0</v>
@@ -27977,7 +29699,7 @@
         <v>0</v>
       </c>
       <c r="BH290" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="BM290">
         <v>0</v>

</xml_diff>

<commit_message>
Kingdom Update Service is fully tested.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/quest-items.xlsx
+++ b/resources/data-imports/Items/quest-items.xlsx
@@ -7545,21 +7545,9 @@
       <c r="AM54">
         <v>0</v>
       </c>
-      <c r="AS54">
-        <v>0</v>
-      </c>
       <c r="AV54">
         <v>0</v>
       </c>
-      <c r="AX54">
-        <v>0</v>
-      </c>
-      <c r="AY54">
-        <v>0</v>
-      </c>
-      <c r="BA54">
-        <v>0</v>
-      </c>
       <c r="BB54">
         <v>0</v>
       </c>
@@ -7577,6 +7565,9 @@
       </c>
       <c r="BG54">
         <v>0</v>
+      </c>
+      <c r="BH54" t="s">
+        <v>182</v>
       </c>
       <c r="BM54">
         <v>0</v>
@@ -28671,7 +28662,19 @@
       <c r="AM279">
         <v>0</v>
       </c>
+      <c r="AS279">
+        <v>0</v>
+      </c>
       <c r="AV279">
+        <v>0</v>
+      </c>
+      <c r="AX279">
+        <v>0</v>
+      </c>
+      <c r="AY279">
+        <v>0</v>
+      </c>
+      <c r="BA279">
         <v>0</v>
       </c>
       <c r="BB279">

</xml_diff>